<commit_message>
combat is now working, but produces some unwanted nulls.
</commit_message>
<xml_diff>
--- a/app/resources/Weapon_Attack_Factors.xlsx
+++ b/app/resources/Weapon_Attack_Factors.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="23955" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="100" windowWidth="23960" windowHeight="11840"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon_Attack_Factors" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" iterate="1"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>classification</t>
   </si>
@@ -61,10 +66,55 @@
     <t>claymore</t>
   </si>
   <si>
-    <t>hand_axe</t>
-  </si>
-  <si>
     <t>battle_axe</t>
+  </si>
+  <si>
+    <t>base_round_time</t>
+  </si>
+  <si>
+    <t>minimum_round_time</t>
+  </si>
+  <si>
+    <t>handaxe</t>
+  </si>
+  <si>
+    <t>whip</t>
+  </si>
+  <si>
+    <t>blunt_weapons</t>
+  </si>
+  <si>
+    <t>cudgel</t>
+  </si>
+  <si>
+    <t>mace</t>
+  </si>
+  <si>
+    <t>morning_star</t>
+  </si>
+  <si>
+    <t>flail</t>
+  </si>
+  <si>
+    <t>hammer</t>
+  </si>
+  <si>
+    <t>maul</t>
+  </si>
+  <si>
+    <t>pilum</t>
+  </si>
+  <si>
+    <t>polearm_weapons</t>
+  </si>
+  <si>
+    <t>spear</t>
+  </si>
+  <si>
+    <t>halberd</t>
+  </si>
+  <si>
+    <t>trident</t>
   </si>
 </sst>
 </file>
@@ -403,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,8 +486,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -462,8 +518,14 @@
       <c r="H2">
         <v>-20</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -488,8 +550,14 @@
       <c r="H3">
         <v>-18</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -514,8 +582,14 @@
       <c r="H4">
         <v>-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -540,8 +614,14 @@
       <c r="H5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -566,8 +646,14 @@
       <c r="H6">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -592,8 +678,14 @@
       <c r="H7">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -618,10 +710,16 @@
       <c r="H8">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -644,10 +742,16 @@
       <c r="H9">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -670,8 +774,371 @@
       <c r="H10">
         <v>25</v>
       </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>35</v>
+      </c>
+      <c r="D11">
+        <v>35</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>17</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>24</v>
+      </c>
+      <c r="H12">
+        <v>17</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>31</v>
+      </c>
+      <c r="G13">
+        <v>34</v>
+      </c>
+      <c r="H13">
+        <v>24</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>33</v>
+      </c>
+      <c r="E14">
+        <v>33</v>
+      </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>34</v>
+      </c>
+      <c r="H14">
+        <v>25</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <v>23</v>
+      </c>
+      <c r="G15">
+        <v>27</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>28</v>
+      </c>
+      <c r="F16">
+        <v>28</v>
+      </c>
+      <c r="G16">
+        <v>33</v>
+      </c>
+      <c r="H16">
+        <v>25</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <v>30</v>
+      </c>
+      <c r="F17">
+        <v>34</v>
+      </c>
+      <c r="G17">
+        <v>38</v>
+      </c>
+      <c r="H17">
+        <v>27</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>25</v>
+      </c>
+      <c r="F18">
+        <v>18</v>
+      </c>
+      <c r="G18">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>33</v>
+      </c>
+      <c r="E19">
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <v>28</v>
+      </c>
+      <c r="H19">
+        <v>21</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>28</v>
+      </c>
+      <c r="F20">
+        <v>27</v>
+      </c>
+      <c r="G20">
+        <v>24</v>
+      </c>
+      <c r="H20">
+        <v>20</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <v>29</v>
+      </c>
+      <c r="E21">
+        <v>28</v>
+      </c>
+      <c r="F21">
+        <v>26</v>
+      </c>
+      <c r="G21">
+        <v>29</v>
+      </c>
+      <c r="H21">
+        <v>13</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>